<commit_message>
Update PCB + PCB with ground plane
</commit_message>
<xml_diff>
--- a/2020-2021/PCB/PCB_Version_2/BOM_PCB_VERSION_2.xlsx
+++ b/2020-2021/PCB/PCB_Version_2/BOM_PCB_VERSION_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11701130\Desktop\PEm\intelliflow\2020-2021\PCB\PCB_Version_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20F70D6-9D7D-4377-B72A-69350564DC68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB3AAAC-474E-4F4C-91AC-6D0CB38B670B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2460" windowWidth="21840" windowHeight="13140" xr2:uid="{5999F184-5D91-49CA-8EEC-480CE4902DE2}"/>
   </bookViews>
@@ -195,15 +195,6 @@
     <t>DC-Power socket</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Switchcraft/RAPC712BKZ?qs=vLWxofP3U2y1tV3BP2KpWw%3D%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAPC712BKZ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">502-RAPC712BKZ </t>
-  </si>
-  <si>
     <t>IC</t>
   </si>
   <si>
@@ -258,6 +249,15 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/KOA-Speer/RN732ATTD5000B25?qs=sGAEpiMZZMtlubZbdhIBIFsbc394gO9GFKU7OCwB87Q%3D</t>
+  </si>
+  <si>
+    <t>PJ-002BH</t>
+  </si>
+  <si>
+    <t>490-PJ-002BH</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/CUI-Devices/PJ-002BH?qs=WyjlAZoYn51nOX1h%2FqpLlg%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -749,7 +749,7 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -861,7 +861,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -897,13 +897,13 @@
         <v>40</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E8" s="1">
         <v>2.64</v>
@@ -917,7 +917,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -973,35 +973,35 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
-        <v>54</v>
+      <c r="B11" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" t="s">
-        <v>55</v>
+        <v>70</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="E11" s="1">
-        <v>1.63</v>
+        <v>0.627</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" ref="G11" si="4">E11*F11</f>
-        <v>1.63</v>
+        <v>0.627</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
         <v>50</v>
@@ -1124,16 +1124,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" t="s">
-        <v>70</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E17" s="1">
         <v>0.71399999999999997</v>
@@ -1151,11 +1151,11 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G19" s="10">
         <f>SUM(G2:G17)</f>
-        <v>49.578000000000003</v>
+        <v>48.575000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1164,10 +1164,9 @@
     <hyperlink ref="C2" r:id="rId1" location="description" xr:uid="{8D06DD26-70E7-4AF9-B0A0-81AB27F2CFEB}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{CE6BE5A4-0CCE-4CFC-A504-483A76E67CC9}"/>
     <hyperlink ref="C9" r:id="rId3" xr:uid="{F4743BE3-3A8D-47E8-AC8C-051509EAF94B}"/>
-    <hyperlink ref="C11" r:id="rId4" xr:uid="{A2C43423-BC5B-4670-8F41-456E8A570AAE}"/>
-    <hyperlink ref="C16" r:id="rId5" xr:uid="{B4DF5C32-D464-4CDA-8AE1-BE6309CED587}"/>
+    <hyperlink ref="C16" r:id="rId4" xr:uid="{B4DF5C32-D464-4CDA-8AE1-BE6309CED587}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>